<commit_message>
Changed names in test case files for anonymity. Redid test cases in TestInteraction.java.
</commit_message>
<xml_diff>
--- a/SocialNetwork/src/test/resources/incites/data/times_cited_multiple_pub.xlsx
+++ b/SocialNetwork/src/test/resources/incites/data/times_cited_multiple_pub.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SloGGy\Documents\Eclipse\SocialNetworkApp\SocialNetwork\src\test\resources\incites\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2740" windowWidth="24560" windowHeight="16220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1725" yWindow="2745" windowWidth="24555" windowHeight="16215" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Logic Tree" sheetId="1" r:id="rId1"/>
@@ -27,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>REHABILITATION</t>
-  </si>
-  <si>
-    <t>Trentham, Barry (UNIV TORONTO); Trentham, Barry (UNIV TORONTO); Dunal, Lynda (UNIV TORONTO); Dunal, Lynda (UNIV TORONTO)</t>
-  </si>
-  <si>
-    <t>Identifying occupational performance issues with older adults: Therapists perspectives</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Times Cited</t>
   </si>
@@ -56,18 +52,29 @@
     <t>Document Title</t>
   </si>
   <si>
-    <t>Trentham, Barry (UNIV TORONTO); Trentham, Barry (UNIV TORONTO); Jack, Tinfoil (UNIV BEANSTALK);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Sisko, Benjamin (UNITED FEDERATION OF PLANETS); Sisko, Benjamin (UNITED FEDERATION OF PLANETS); Bashir, Julian (UNITED FEDERATION OF PLANETS); Bashir, Julian (UNITED FEDERATION OF PLANETS)</t>
+  </si>
+  <si>
+    <t>Sisko, Benjamin (UNITED FEDERATION OF PLANETS); Sisko, Benjamin (UNITED FEDERATION OF PLANETS); Nerys, Kira (UNIV OF BAJOR);</t>
+  </si>
+  <si>
+    <t>DEEP SPACE NINE</t>
+  </si>
+  <si>
+    <t>Key improvements resulting from the continued presence of the Federation in Bajor</t>
+  </si>
+  <si>
+    <t>Frontier Medicine: A report documenting the trials and tribulations of medical practice in Deep Space Nine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -165,6 +172,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,17 +502,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -507,17 +521,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -527,36 +540,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="27.375" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39">
+    <row r="1" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="168">
+    <row r="2" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -567,16 +584,16 @@
         <v>2009</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="126">
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>7</v>
       </c>
@@ -587,20 +604,19 @@
         <v>2009</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -610,17 +626,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -630,17 +645,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -650,17 +664,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -670,17 +683,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -690,17 +702,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -710,17 +721,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>